<commit_message>
Fixed duplicated entries for Enquiry bug.
</commit_message>
<xml_diff>
--- a/data/Enquiries.xlsx
+++ b/data/Enquiries.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
   <si>
     <t>Enquiry ID</t>
   </si>
@@ -80,7 +80,7 @@
     <t>2025-04-23T13:25:58.717511</t>
   </si>
   <si>
-    <t>Yeah it worked!</t>
+    <t>Yes I can see this!</t>
   </si>
   <si>
     <t>S5678901G</t>
@@ -89,7 +89,13 @@
     <t>Manager</t>
   </si>
   <si>
-    <t>2025-04-23T14:23:44.511042</t>
+    <t>2025-04-23T15:26:51.459171</t>
+  </si>
+  <si>
+    <t>How about you?</t>
+  </si>
+  <si>
+    <t>2025-04-23T15:27:06.254456</t>
   </si>
 </sst>
 </file>
@@ -134,7 +140,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -281,45 +287,19 @@
         <v>19</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="G6" t="s" s="0">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="H6" t="s" s="0">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="E7" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="F7" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="G7" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="H7" t="s" s="0">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed BTORepository and UserRepository initialization to singleton call.
</commit_message>
<xml_diff>
--- a/data/Enquiries.xlsx
+++ b/data/Enquiries.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="32">
   <si>
     <t>Enquiry ID</t>
   </si>
@@ -96,6 +96,18 @@
   </si>
   <si>
     <t>2025-04-23T15:27:06.254456</t>
+  </si>
+  <si>
+    <t>Are you there?</t>
+  </si>
+  <si>
+    <t>2025-04-23T23:06:54.954202</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>2025-04-23T23:07:20.782654</t>
   </si>
 </sst>
 </file>
@@ -140,7 +152,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -302,6 +314,58 @@
         <v>27</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="G7" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="H7" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="G8" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="H8" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>